<commit_message>
Compressed Rule Management API's
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/REGION.xlsx
+++ b/Lexis-GLOBAL/Coredata/REGION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI_AdminPortal\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C50FC-2CB4-4EF8-BE6A-91DAA8442614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5A6590-448C-4C4D-8D6E-0E8C550153E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_Create" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="71">
   <si>
     <t>S.No</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Inprogress</t>
   </si>
   <si>
     <t>New</t>
@@ -693,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F83A6FB-A034-4DD8-86B8-CFDDCA5856F5}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -746,19 +743,19 @@
         <v>21</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>8</v>
@@ -790,7 +787,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -844,13 +841,13 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -883,10 +880,10 @@
         <v>14</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>17</v>
@@ -904,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
@@ -943,10 +940,10 @@
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>17</v>
@@ -964,13 +961,13 @@
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
@@ -1003,10 +1000,10 @@
         <v>14</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>17</v>
@@ -1024,13 +1021,13 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
@@ -1063,10 +1060,10 @@
         <v>14</v>
       </c>
       <c r="Q6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>17</v>
@@ -1084,13 +1081,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>18</v>
@@ -1123,10 +1120,10 @@
         <v>14</v>
       </c>
       <c r="Q7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>17</v>
@@ -1195,19 +1192,19 @@
         <v>21</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>8</v>
@@ -1230,7 +1227,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>13</v>
@@ -1239,7 +1236,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>18</v>
@@ -1290,16 +1287,16 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>18</v>
@@ -1332,10 +1329,10 @@
         <v>14</v>
       </c>
       <c r="Q3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>17</v>
@@ -1350,16 +1347,16 @@
         <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>18</v>
@@ -1392,10 +1389,10 @@
         <v>14</v>
       </c>
       <c r="Q4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>17</v>
@@ -1410,16 +1407,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>18</v>
@@ -1452,10 +1449,10 @@
         <v>14</v>
       </c>
       <c r="Q5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>17</v>
@@ -1470,16 +1467,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>18</v>
@@ -1512,10 +1509,10 @@
         <v>14</v>
       </c>
       <c r="Q6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>17</v>
@@ -1530,16 +1527,16 @@
         <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>18</v>
@@ -1572,10 +1569,10 @@
         <v>14</v>
       </c>
       <c r="Q7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>17</v>
@@ -1645,19 +1642,19 @@
         <v>21</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>8</v>
@@ -1680,7 +1677,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
@@ -1689,7 +1686,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -1740,16 +1737,16 @@
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -1782,10 +1779,10 @@
         <v>14</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>17</v>
@@ -1800,16 +1797,16 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
@@ -1842,10 +1839,10 @@
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>17</v>
@@ -1860,16 +1857,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
@@ -1902,10 +1899,10 @@
         <v>14</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>17</v>
@@ -1920,16 +1917,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
@@ -1962,10 +1959,10 @@
         <v>14</v>
       </c>
       <c r="Q6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>17</v>
@@ -1980,16 +1977,16 @@
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>18</v>
@@ -2022,10 +2019,10 @@
         <v>14</v>
       </c>
       <c r="Q7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>17</v>
@@ -2034,7 +2031,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2099,19 +2096,19 @@
         <v>21</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>8</v>
@@ -2134,7 +2131,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
@@ -2143,7 +2140,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -2194,16 +2191,16 @@
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -2236,10 +2233,10 @@
         <v>14</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>17</v>
@@ -2254,16 +2251,16 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
@@ -2296,10 +2293,10 @@
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>17</v>
@@ -2314,16 +2311,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
@@ -2356,10 +2353,10 @@
         <v>14</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>17</v>
@@ -2374,16 +2371,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
@@ -2416,10 +2413,10 @@
         <v>14</v>
       </c>
       <c r="Q6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>17</v>
@@ -2434,16 +2431,16 @@
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>18</v>
@@ -2476,10 +2473,10 @@
         <v>14</v>
       </c>
       <c r="Q7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>17</v>
@@ -2560,19 +2557,19 @@
         <v>21</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>8</v>
@@ -2595,7 +2592,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
@@ -2604,7 +2601,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -2655,16 +2652,16 @@
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -2697,10 +2694,10 @@
         <v>14</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>17</v>
@@ -2715,16 +2712,16 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
@@ -2757,10 +2754,10 @@
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>17</v>
@@ -2775,16 +2772,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
@@ -2817,10 +2814,10 @@
         <v>14</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>17</v>
@@ -2835,16 +2832,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
@@ -2877,10 +2874,10 @@
         <v>14</v>
       </c>
       <c r="Q6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>17</v>
@@ -2895,16 +2892,16 @@
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>18</v>
@@ -2937,10 +2934,10 @@
         <v>14</v>
       </c>
       <c r="Q7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>17</v>
@@ -2956,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DF612-9D63-4DEA-BCA2-55F7199572F3}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2985,7 +2982,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -2996,7 +2993,7 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3007,7 +3004,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3018,7 +3015,7 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3029,7 +3026,7 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3040,7 +3037,7 @@
         <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3051,7 +3048,7 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3062,7 +3059,7 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3073,7 +3070,7 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3081,10 +3078,10 @@
         <v>33</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3092,10 +3089,10 @@
         <v>34</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -3103,10 +3100,10 @@
         <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -3114,10 +3111,10 @@
         <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3125,7 +3122,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3133,7 +3130,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="15"/>
     </row>
@@ -3145,10 +3142,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="G19" s="15"/>
     </row>

</xml_diff>